<commit_message>
Make last enhancements accord to review
</commit_message>
<xml_diff>
--- a/example_wine_database.xlsx
+++ b/example_wine_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonchik\!devman progs\projects\wine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41ECC8-5E4C-4F70-A239-E578ED2C0651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78066AA3-F71F-4FB1-AA17-B20D100B2E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,10 +402,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -594,6 +594,13 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>